<commit_message>
add per-wall damage, flood duration, Observer Name, and strict naming rules
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1601,6 +1601,146 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Wall Damage % (Front)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Analyze "front" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Wall Damage % (Rear)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Analyze "rear" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Wall Damage % (Left)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Analyze "left" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Wall Damage % (Right)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Analyze "right" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Flood Duration (Hours)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Numeric</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Check specific reports or interviews. Very hard to tell visually. Likely [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
revert to cardinal directions (North/South/East/West) for wall damage
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -1605,27 +1605,27 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Wall Damage % (Front)</t>
+          <t>Flood Duration (Hours)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
+          <t>Numeric</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Analyze "front" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+          <t>Check specific reports or interviews. Very hard to tell visually. Likely [NEEDS_RESEARCH].</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Flood</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Wall Damage % (Rear)</t>
+          <t>Wall Damage % (North)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Analyze "rear" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+          <t>Analyze "north" images. Estimate % wall failure. If no `north_` image, use [NEEDS_RESEARCH].</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1661,7 +1661,7 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Wall Damage % (Left)</t>
+          <t>Wall Damage % (South)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Analyze "left" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+          <t>Analyze "south" images. Estimate % wall failure. If no `south_` image, use [NEEDS_RESEARCH].</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1689,7 +1689,7 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Wall Damage % (Right)</t>
+          <t>Wall Damage % (East)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Analyze "right" images. Estimate % wall failure. If obscured/missing, use [NEEDS_RESEARCH].</t>
+          <t>Analyze "east" images. Estimate % wall failure. If no `east_` image, use [NEEDS_RESEARCH].</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1717,27 +1717,27 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Flood Duration (Hours)</t>
+          <t>Wall Damage % (West)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Numeric</t>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Check specific reports or interviews. Very hard to tell visually. Likely [NEEDS_RESEARCH].</t>
+          <t>Analyze "west" images. Estimate % wall failure. If no `west_` image, use [NEEDS_RESEARCH].</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>All</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reorganize schema into logical groupings and clean up report header
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,12 +440,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Attribute Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Type</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Attribute Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -472,12 +472,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Property ID</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>ID</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Property ID</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -500,12 +500,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Property Name</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>ID</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Property Name</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -530,12 +530,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>National Register ID</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>ID</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>National Register ID</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -560,12 +560,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Archetype Number</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Archetype Number</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -590,12 +590,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Archetype Description</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Archetype Description</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -620,12 +620,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Pre-Event Status</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Pre-Event Status</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -650,12 +650,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Significance Type</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Significance Type</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -680,12 +680,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Construction Year</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Construction Year</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -710,22 +710,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Number of Stories</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Structural Wall System</t>
-        </is>
-      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>URM (Brick), URM (Stone), URM (Concrete), Hybrid, Wood Frame</t>
+          <t>1, 1.5, 2, 3, 4, 5, 6+</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Look for header rows (sideways bricks) indicating multi-wythe structural URM.</t>
+          <t>Count horizontal window rows from street-level imagery.</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
@@ -740,22 +740,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Urban Setting</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Wall Anchorage Type</t>
-        </is>
-      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>None, Star/S-Plates, Punched Plates, Through-Bolts, Iron Straps</t>
+          <t>Urban, Suburban, Rural</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Identify metal hardware at floor or roof lines on "Before" facades.</t>
+          <t>Assess density and proximity to neighbors in "Before" satellite view.</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
@@ -770,22 +770,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Building Position</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Masonry Leaves</t>
-        </is>
-      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4+ Wythes</t>
+          <t>Corner, Mid-block, End-of-block</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Check window depth or corner exposures in technical documentation.</t>
+          <t>Determine position relative to intersections from map data.</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
@@ -800,22 +800,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Structural Wall System</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Wall Thickness</t>
-        </is>
-      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Numeric (inches or mm)</t>
+          <t>URM (Brick), URM (Stone), URM (Concrete), Hybrid, Wood Frame</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Extract from NRHP technical description or floor plans.</t>
+          <t>Look for header rows (sideways bricks) indicating multi-wythe structural URM.</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
@@ -830,22 +830,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Wall Anchorage Type</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Number of Stories</t>
-        </is>
-      </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1, 1.5, 2, 3, 4, 5, 6+</t>
+          <t>None, Star/S-Plates, Punched Plates, Through-Bolts, Iron Straps</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Count horizontal window rows from street-level imagery.</t>
+          <t>Identify metal hardware at floor or roof lines on "Before" facades.</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
@@ -860,22 +860,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Masonry Leaves</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Urban Setting</t>
-        </is>
-      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Urban, Suburban, Rural</t>
+          <t>1, 2, 3, 4+ Wythes</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Assess density and proximity to neighbors in "Before" satellite view.</t>
+          <t>Check window depth or corner exposures in technical documentation.</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
@@ -890,22 +890,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Wall Thickness</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Building Position</t>
-        </is>
-      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Corner, Mid-block, End-of-block</t>
+          <t>Numeric (inches or mm)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Determine position relative to intersections from map data.</t>
+          <t>Extract from NRHP technical description or floor plans.</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
@@ -920,12 +920,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Material (Vertical)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Material (Vertical)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -950,12 +950,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Material (Horizontal)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>Baseline</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Material (Horizontal)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -980,26 +980,26 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Roof System</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>Tornado</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>EF-Rating (Local)</t>
-        </is>
-      </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>EF0, EF1, EF2, EF3, EF4</t>
+          <t>Timber Truss, Heavy Masonry, Steel, Hybrid</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Use NWS/NOAA DAT coordinates to find local intensity at the site.</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
+          <t>Determine based on recon notes or debris visibility in "After" photos.</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>46025</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1010,22 +1010,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Roof Shape &amp; Slope</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>Tornado</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Mechanism of Failure</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Global, Out-of-Plane, Roof-First, Secondary Element</t>
+          <t>Flat, Gable, Hip, Mansard; High, Med, Low slope</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Roof-First = Walls stand, roof missing; Out-of-Plane = Masonry wall collapsed.</t>
+          <t>Analyze geometry from top-down or oblique aerial views.</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
@@ -1040,22 +1040,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Roof-Wall Attachment</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>Tornado</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Roof System</t>
-        </is>
-      </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Timber Truss, Heavy Masonry, Steel, Hybrid</t>
+          <t>Toe-Nail, Bolts, Straps, Hurricane Clips, Unknown</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Determine based on recon notes or debris visibility in "After" photos.</t>
+          <t>Crucial for "Roof-First" failures; check recon/FAST reports.</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
@@ -1070,22 +1070,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Parapet/Overhang</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>Tornado</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Roof Shape &amp; Slope</t>
-        </is>
-      </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Flat, Gable, Hip, Mansard; High, Med, Low slope</t>
+          <t>Numeric (inches/cm)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Analyze geometry from top-down or oblique aerial views.</t>
+          <t>Visually estimate from "Before" oblique imagery or facade photos.</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
@@ -1100,22 +1100,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tornado</t>
+          <t>First-Floor Elevation</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Roof-Wall Attachment</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Toe-Nail, Bolts, Straps, Hurricane Clips, Unknown</t>
+          <t>Numeric (relative to ground)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Crucial for "Roof-First" failures; check recon/FAST reports.</t>
+          <t>Compare threshold of lowest door to adjacent ground grade.</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
@@ -1130,26 +1130,24 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Tornado</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Parapet/Overhang</t>
-        </is>
-      </c>
+          <t>Foundation Condition</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Numeric (inches/cm)</t>
+          <t>Scour, Slab Crack, Shifted, Intact</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Visually estimate from "Before" oblique imagery or facade photos.</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>46025</v>
+          <t>Check for exposed footings (scour), cracks in slab, or movement.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1160,22 +1158,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Door Presence</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>First-Floor Elevation</t>
+          <t>Directional</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Numeric (relative to ground)</t>
+          <t>Large door, Standard door, Not present (N,S,E,W)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Compare threshold of lowest door to adjacent ground grade.</t>
+          <t>Large doors (e.g., fire halls) are high-pressure failure points.</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
@@ -1190,22 +1188,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Protection Present</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Visible Water Line</t>
+          <t>Directional</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Numeric (meters or feet)</t>
+          <t>Shutters, Impact Glass, Plywood, None</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Identify debris lines or horizontal silt stains on the masonry.</t>
+          <t>Check for protective hardware or boards in "After" images.</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
@@ -1220,26 +1218,26 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>EF-Rating (Local)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Masonry Saturation</t>
+          <t>Tornado</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>None, Capillary Rise, Saturated, Efflorescence</t>
+          <t>EF0, EF1, EF2, EF3, EF4</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Capillary Rise = Dark band at base; Efflorescence = White salt stains.</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>46025</v>
+          <t>Use NWS/NOAA DAT coordinates to find local intensity at the site.</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1250,82 +1248,78 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Flood Depth (Visible)</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Numeric (feet/cm)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Measure height of mudline relative to windows/doors if visible.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
           <t>Flood</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Mortar Condition</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Crumbly/Sandy, Hard, Missing, Intact</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Zoom into high-res "After" photos to check for joint erosion/voids.</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>46025</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>All</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Directional</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Wall Damage (N,S,E,W)</t>
-        </is>
-      </c>
+          <t>Flood Duration (Hours)</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Undamaged, Minor, Moderate, Severe, Destroyed</t>
+          <t>Numeric</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Assess each facade separately; look for cracks, bowing, or collapse.</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>46025</v>
+          <t>Check specific reports or interviews. Very hard to tell visually. Likely [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Flood</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Directional</t>
+          <t>Mechanism of Failure</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Wall Structure Damage</t>
+          <t>Tornado</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Damage to structural wythes (N,S,E,W)</t>
+          <t>Global, Out-of-Plane, Roof-First, Secondary Element</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Identifies if the load-bearing mass failed vs. just surface finish.</t>
+          <t>Roof-First = Walls stand, roof missing; Out-of-Plane = Masonry wall collapsed.</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
@@ -1340,26 +1334,24 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Directional</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Substrate/Cladding</t>
-        </is>
-      </c>
+          <t>Roof Damage %</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Damage to veneer/outer wythe (N,S,E,W)</t>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Identifies surface-only damage (e.g., loss of brick face or siding).</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>46025</v>
+          <t>Estimate percentage of roof covering missing or structure failed.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1370,26 +1362,24 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Directional</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Fenestration Status</t>
-        </is>
-      </c>
+          <t>Wall Damage % (North)</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>% Broken/Damaged per facade (N,S,E,W)</t>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Percent of window/door area that is failed or missing.</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>46025</v>
+          <t>Analyze "north" images. Estimate % wall failure. If no `north_` image, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1400,26 +1390,24 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Directional</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Protection Present</t>
-        </is>
-      </c>
+          <t>Wall Damage % (South)</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Shutters, Impact Glass, Plywood, None</t>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Check for protective hardware or boards in "After" images.</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>46025</v>
+          <t>Analyze "south" images. Estimate % wall failure. If no `south_` image, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1430,26 +1418,24 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Directional</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Door Presence</t>
-        </is>
-      </c>
+          <t>Wall Damage % (East)</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Large door, Standard door, Not present (N,S,E,W)</t>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Large doors (e.g., fire halls) are high-pressure failure points.</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>46025</v>
+          <t>Analyze "east" images. Estimate % wall failure. If no `east_` image, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1460,26 +1446,24 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Recovery</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Building Use Plan</t>
-        </is>
-      </c>
+          <t>Wall Damage % (West)</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Demolished, Rededicated, Restored, Abandoned</t>
+          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Compare imagery from 1-3 years post-event to determine outcome.</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>46025</v>
+          <t>Analyze "west" images. Estimate % wall failure. If no `west_` image, use [NEEDS_RESEARCH].</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1490,252 +1474,238 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>Visible Water Line</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Numeric (meters or feet)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Identify debris lines or horizontal silt stains on the masonry.</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Masonry Saturation</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>None, Capillary Rise, Saturated, Efflorescence</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Capillary Rise = Dark band at base; Efflorescence = White salt stains.</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Mortar Condition</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Crumbly/Sandy, Hard, Missing, Intact</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Zoom into high-res "After" photos to check for joint erosion/voids.</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Wall Structure Damage</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Directional</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Damage to structural wythes (N,S,E,W)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Identifies if the load-bearing mass failed vs. just surface finish.</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Substrate/Cladding</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Directional</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Damage to veneer/outer wythe (N,S,E,W)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Identifies surface-only damage (e.g., loss of brick face or siding).</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Fenestration Status</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Directional</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>% Broken/Damaged per facade (N,S,E,W)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Percent of window/door area that is failed or missing.</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Building Use Plan</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Recovery</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Demolished, Rededicated, Restored, Abandoned</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Compare imagery from 1-3 years post-event to determine outcome.</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Existence (Multi-yr)</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>Timeline</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Existence (Multi-yr)</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>Binary (Yes/No) for -5 to +5 years</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Track presence of the structure using multi-year historic aerials.</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E43" s="2" t="n">
         <v>46024</v>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr"/>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Foundation Condition</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Scour, Slab Crack, Shifted, Intact</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Check for exposed footings (scour), cracks in slab, or movement.</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Roof Damage %</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Estimate percentage of roof covering missing or structure failed.</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr"/>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Flood Depth (Visible)</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Numeric (feet/cm)</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Measure height of mudline relative to windows/doors if visible.</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Flood</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr"/>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Flood Duration (Hours)</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Numeric</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Check specific reports or interviews. Very hard to tell visually. Likely [NEEDS_RESEARCH].</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Flood</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr"/>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Wall Damage % (North)</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Analyze "north" images. Estimate % wall failure. If no `north_` image, use [NEEDS_RESEARCH].</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr"/>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Wall Damage % (South)</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Analyze "south" images. Estimate % wall failure. If no `south_` image, use [NEEDS_RESEARCH].</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Wall Damage % (East)</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Analyze "east" images. Estimate % wall failure. If no `east_` image, use [NEEDS_RESEARCH].</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
       <c r="F43" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Wall Damage % (West)</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>0%, &lt;25%, 25-50%, 50-75%, &gt;75%</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Analyze "west" images. Estimate % wall failure. If no `west_` image, use [NEEDS_RESEARCH].</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
         <is>
           <t>All</t>
         </is>

</xml_diff>

<commit_message>
fix corrupted features schema and fully restore sample report data
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -490,7 +486,11 @@
           <t>Use the folder name assigned in OneDrive; this is the primary key.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>All</t>
@@ -518,8 +518,10 @@
           <t>Search NRHP database by property address or name.</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>46025</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -548,8 +550,10 @@
           <t>Search NRHP database by address or name.</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>1</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -578,8 +582,10 @@
           <t>See archetypes spreadsheet</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>46025</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -608,8 +614,10 @@
           <t>Describe building use based on "Before" signage and architectural style.</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>46025</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -638,8 +646,10 @@
           <t>Look for "Before" clues like boarded windows (mothballed) vs. signage (active).</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>46025</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -668,8 +678,10 @@
           <t>Extracted from the NRHP nomination narrative text.</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>1</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -698,8 +710,10 @@
           <t>Use year listed in NRHP/Property Cards; estimate by style if missing.</t>
         </is>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>46025</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -728,8 +742,10 @@
           <t>Count horizontal window rows from street-level imagery.</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>46025</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -758,8 +774,10 @@
           <t>Assess density and proximity to neighbors in "Before" satellite view.</t>
         </is>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>46025</v>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -788,8 +806,10 @@
           <t>Determine position relative to intersections from map data.</t>
         </is>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>46025</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -818,8 +838,10 @@
           <t>Look for header rows (sideways bricks) indicating multi-wythe structural URM.</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>46025</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -848,8 +870,10 @@
           <t>Identify metal hardware at floor or roof lines on "Before" facades.</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>46025</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -878,8 +902,10 @@
           <t>Check window depth or corner exposures in technical documentation.</t>
         </is>
       </c>
-      <c r="E15" s="2" t="n">
-        <v>46025</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -908,8 +934,10 @@
           <t>Extract from NRHP technical description or floor plans.</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>46025</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -938,8 +966,10 @@
           <t>Identify the primary facade load-bearing material.</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>46025</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -968,8 +998,10 @@
           <t>Extract from recon reports; often timber in older historic buildings.</t>
         </is>
       </c>
-      <c r="E18" s="2" t="n">
-        <v>46025</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -998,8 +1030,10 @@
           <t>Determine based on recon notes or debris visibility in "After" photos.</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>46025</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1028,8 +1062,10 @@
           <t>Analyze geometry from top-down or oblique aerial views.</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>46025</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1058,8 +1094,10 @@
           <t>Crucial for "Roof-First" failures; check recon/FAST reports.</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
-        <v>46025</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1088,8 +1126,10 @@
           <t>Visually estimate from "Before" oblique imagery or facade photos.</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
-        <v>46025</v>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1118,8 +1158,10 @@
           <t>Compare threshold of lowest door to adjacent ground grade.</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>46025</v>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1176,8 +1218,10 @@
           <t>Large doors (e.g., fire halls) are high-pressure failure points.</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
-        <v>46025</v>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1206,8 +1250,10 @@
           <t>Check for protective hardware or boards in "After" images.</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
-        <v>46025</v>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1236,8 +1282,10 @@
           <t>Use NWS/NOAA DAT coordinates to find local intensity at the site.</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>1</v>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1322,8 +1370,10 @@
           <t>Roof-First = Walls stand, roof missing; Out-of-Plane = Masonry wall collapsed.</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
-        <v>46025</v>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1492,8 +1542,10 @@
           <t>Identify debris lines or horizontal silt stains on the masonry.</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>46025</v>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1522,8 +1574,10 @@
           <t>Capillary Rise = Dark band at base; Efflorescence = White salt stains.</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
-        <v>46025</v>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1552,8 +1606,10 @@
           <t>Zoom into high-res "After" photos to check for joint erosion/voids.</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>46025</v>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1582,8 +1638,10 @@
           <t>Identifies if the load-bearing mass failed vs. just surface finish.</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>46025</v>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1612,8 +1670,10 @@
           <t>Identifies surface-only damage (e.g., loss of brick face or siding).</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>46025</v>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1642,8 +1702,10 @@
           <t>Percent of window/door area that is failed or missing.</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>46025</v>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1672,8 +1734,10 @@
           <t>Compare imagery from 1-3 years post-event to determine outcome.</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
-        <v>46025</v>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1702,8 +1766,10 @@
           <t>Track presence of the structure using multi-year historic aerials.</t>
         </is>
       </c>
-      <c r="E43" s="2" t="n">
-        <v>46024</v>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>

</xml_diff>